<commit_message>
updated to fetch data from actual product file
</commit_message>
<xml_diff>
--- a/static/lips_loreal.xlsx
+++ b/static/lips_loreal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NexusMacBookProYeo/Desktop/Y4S1/BT4103 - Capstone/capstone cv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu-my.sharepoint.com/personal/e0543650_u_nus_edu/Documents/Strudy/Y4S1/Capstone/capstone/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3512D7D6-86B5-F746-8BED-A250DA48A0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -866,15 +866,15 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,7 +891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -911,7 +911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -931,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -951,7 +951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -971,7 +971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -991,7 +991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>

</xml_diff>